<commit_message>
boxes added, spectrum created
</commit_message>
<xml_diff>
--- a/clean data.xlsx
+++ b/clean data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nurgu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workbench\TV_fm_dri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{65E6ED27-70FC-4420-8C72-F2686EF381D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427749FC-92A7-455B-8986-0407FE2E4A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{745014C1-4A07-4CC1-9D94-6351EACBA71E}"/>
   </bookViews>
@@ -1165,42 +1165,13 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Aptos"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Aptos"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1515,6 +1486,35 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1529,30 +1529,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{246F6817-EF5D-42D2-BFE5-280A7132B0D0}" name="Table1" displayName="Table1" ref="A1:U292" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{246F6817-EF5D-42D2-BFE5-280A7132B0D0}" name="Table1" displayName="Table1" ref="A1:U292" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:U292" xr:uid="{08C4E2AE-4885-43DC-8611-35864C93CA5D}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="İndeks" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Tezlik istifadəçisi" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Yayım növü(TV, RY)" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Quraşdırılma ünvanı" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Avadanlığın tipi və modeli" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="KOORDİNAT Uzunluq dairəsi  (DEC)  N" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="KOORDİNAT En dairəsi (DEC)  E" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Tezlik, MHs" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Kanal" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Çıxış gücüVt" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Polyarizasiya" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Zolaq eni, MHs" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Antenin asılma hündürlüyü, H (m)" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Antenna güclənmə əmsalıdB" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Effektiv antena hündürlüyü" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Proqramın qəbul üsulu" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Boşaldılacaq kanallar" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Radio/TV" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Tezlik kateqoriyasi" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Yayım kateqoriyası" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Rayon" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="İndeks" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Tezlik istifadəçisi" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Yayım növü(TV, RY)" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Quraşdırılma ünvanı" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Avadanlığın tipi və modeli" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="KOORDİNAT Uzunluq dairəsi  (DEC)  N" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="KOORDİNAT En dairəsi (DEC)  E" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Tezlik, MHs" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Kanal" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Çıxış gücüVt" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Polyarizasiya" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Zolaq eni, MHs" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Antenin asılma hündürlüyü, H (m)" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Antenna güclənmə əmsalıdB" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Effektiv antena hündürlüyü" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Proqramın qəbul üsulu" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Boşaldılacaq kanallar" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Radio/TV" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Tezlik kateqoriyasi" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Yayım kateqoriyası" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Rayon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1878,7 +1878,7 @@
   <dimension ref="A1:U292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="S287" sqref="S287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -20536,7 +20536,7 @@
         <v>183</v>
       </c>
       <c r="R287" s="1" t="s">
-        <v>147</v>
+        <v>25</v>
       </c>
       <c r="S287" s="1" t="s">
         <v>29</v>

</xml_diff>